<commit_message>
final project test code
</commit_message>
<xml_diff>
--- a/final/result.xlsx
+++ b/final/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\MLFN\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA866D42-BA9E-4FAE-9EED-913BB4681083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B193429-B37B-48CB-8E8E-D387C1D074D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2C4E1AD5-ECD5-4651-8BB2-064DAA27BDD5}"/>
   </bookViews>
@@ -89,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.0000"/>
+    <numFmt numFmtId="176" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -134,57 +134,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2633,16 +2590,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>158115</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>89534</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>339090</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>253365</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>116205</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2669,16 +2626,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>175258</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>167641</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>45719</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>200026</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3006,7 +2963,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>

</xml_diff>